<commit_message>
add sc study (2018.02.11)
</commit_message>
<xml_diff>
--- a/certificate/sc-japan/과거문제정리.xlsx
+++ b/certificate/sc-japan/과거문제정리.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t>경과</t>
     <phoneticPr fontId="3"/>
@@ -67,14 +67,6 @@
   </si>
   <si>
     <t>패스함</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2013 봄</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2013 가을</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
@@ -2461,27 +2453,15 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
+    <t>10</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
     <t>12</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>6</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>7</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>8</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>9</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>11</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
@@ -2949,7 +2929,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3085,9 +3065,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3152,6 +3129,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3438,10 +3421,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L296"/>
+  <dimension ref="A1:L294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3458,132 +3441,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="B1" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="61" t="s">
+      <c r="B1" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="66"/>
+      <c r="F1" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="66"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3"/>
-      <c r="B2" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="59" t="s">
+      <c r="B2" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="E2" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="F2" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="G2" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="H2" s="57" t="s">
         <v>63</v>
       </c>
+      <c r="I2" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="61" t="s">
+      <c r="B3" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="C3" s="62"/>
+      <c r="D3" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="E3" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="59" t="s">
+      <c r="F3" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="58" t="s">
+      <c r="G3" s="59" t="s">
         <v>56</v>
       </c>
+      <c r="H3" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:11" s="41" customFormat="1">
-      <c r="A4" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="55" t="s">
+      <c r="A4" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="B4" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="C4" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="D4" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="E4" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="F4" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="G4" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="H4" s="50" t="s">
         <v>46</v>
       </c>
+      <c r="I4" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="K4" s="42"/>
     </row>
     <row r="5" spans="1:11" s="41" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A5" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="47" t="s">
+      <c r="A5" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="B5" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="45"/>
+      <c r="C5" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="67"/>
+      <c r="G5" s="68"/>
       <c r="H5" s="43"/>
       <c r="I5" s="44"/>
       <c r="J5" s="43"/>
@@ -3591,136 +3574,136 @@
     </row>
     <row r="6" spans="1:11" ht="61.5" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" s="36"/>
       <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:11" ht="60" customHeight="1">
       <c r="A7" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="34"/>
       <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:11" ht="59.25" customHeight="1">
       <c r="A8" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:11" ht="64.5" customHeight="1">
       <c r="A9" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="67.5" customHeight="1">
       <c r="A10" s="27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="24"/>
@@ -3730,11 +3713,11 @@
     </row>
     <row r="11" spans="1:11" ht="67.5" customHeight="1">
       <c r="A11" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>4</v>
@@ -3747,171 +3730,147 @@
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:11" ht="67.5" customHeight="1">
-      <c r="A12" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="20" t="s">
+      <c r="A12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:11" ht="67.5" customHeight="1">
-      <c r="A13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:11" ht="67.5" customHeight="1">
-      <c r="A14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="9"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D16" s="6"/>
+      <c r="E16" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:4">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:4">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:4">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:4">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:4">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:4">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:4">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:4">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:4">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:4">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:4">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:4">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -4061,20 +4020,8 @@
       <c r="C56" s="4"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="296" spans="12:12">
-      <c r="L296" s="2" t="s">
+    <row r="294" spans="12:12">
+      <c r="L294" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>